<commit_message>
floating pt prob added
</commit_message>
<xml_diff>
--- a/data/data-chal/chal3.xlsx
+++ b/data/data-chal/chal3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shevious/workspace/SVAMP_ko/data/data-chal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0642384F-91F1-8943-B2C1-2A05AC494DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80C99F0-4D7B-C643-B54D-DEB4159C7496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8000" yWindow="500" windowWidth="43600" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="149">
   <si>
     <t>Question</t>
   </si>
@@ -520,6 +520,26 @@
   </si>
   <si>
     <t>/ % number3 * number1 number2 number2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떤 소수의 소수점을 오른쪽으로 1 자리 옮기면 원래보다 2.7만큼 커집니다. 원래의 소수를 구하시오.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x*10=x+N1, x = N0/(10.0*N0-1.0)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떤 소수의 소수점을 왼쪽으로 1 자리 옮기면 원래보다 2.7만큼 작아집니다. 원래의 소수를 구하시오.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x/10 = x-N1, x=10x-10*N1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ number1 - * number0 10.0 1.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -899,16 +919,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="107.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="69.5" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
@@ -2421,6 +2441,28 @@
         <v>143</v>
       </c>
     </row>
+    <row r="60" spans="1:11" ht="18">
+      <c r="A60" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="18">
+      <c r="A61" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>